<commit_message>
added HCR toy model
</commit_message>
<xml_diff>
--- a/tables/TableS3_species.xlsx
+++ b/tables/TableS3_species.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/us_fmps/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3116AF4-F856-5B42-89C2-3E1560D82C6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0A7946-074A-A645-B2D8-9731F6183F79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="5600" windowWidth="28040" windowHeight="17440" xr2:uid="{F97615BC-C238-FD4E-A317-C1493B13AD51}"/>
   </bookViews>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3691B0A-AA28-E84B-9AC3-63025FE4CB25}">
   <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4006,6 +4006,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>